<commit_message>
New analysis with keen-eye
</commit_message>
<xml_diff>
--- a/LOR Project_expanded_batuhan_hoca_sunum.xlsx
+++ b/LOR Project_expanded_batuhan_hoca_sunum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\GIT\AURA_REFERENCE_LETTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B93B458-47F6-4738-9356-0312626CE9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC475F7A-DF0F-4649-80C5-B1A51F301767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="203">
   <si>
     <t>Male</t>
   </si>
@@ -693,6 +693,15 @@
   </si>
   <si>
     <t>Letter writer academic rank - Female Applicant- Female Writer</t>
+  </si>
+  <si>
+    <t>Total Writer</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -781,7 +790,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="80">
+  <borders count="89">
     <border>
       <left/>
       <right/>
@@ -1778,6 +1787,137 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1785,7 +1925,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1914,108 +2054,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="73" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2028,6 +2066,170 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="79" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="73" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="80" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="81" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -2476,19 +2678,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P24"/>
+  <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
@@ -2498,59 +2702,59 @@
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="74"/>
-      <c r="C4" s="72" t="s">
+      <c r="B4" s="86"/>
+      <c r="C4" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="89" t="s">
         <v>198</v>
       </c>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="77" t="s">
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="78" t="s">
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="80"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="92"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="75"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="81" t="s">
+      <c r="B5" s="87"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="83" t="s">
+      <c r="E5" s="94"/>
+      <c r="F5" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="84"/>
-      <c r="H5" s="81" t="s">
+      <c r="G5" s="96"/>
+      <c r="H5" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="82"/>
-      <c r="J5" s="83" t="s">
+      <c r="I5" s="94"/>
+      <c r="J5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="84"/>
-      <c r="L5" s="85" t="s">
+      <c r="K5" s="96"/>
+      <c r="L5" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="83" t="s">
+      <c r="M5" s="94"/>
+      <c r="N5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="86"/>
+      <c r="O5" s="98"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="76"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="57" t="s">
         <v>6</v>
       </c>
@@ -3049,12 +3253,160 @@
         <v>66.978922716627594</v>
       </c>
     </row>
+    <row r="22" spans="2:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="136"/>
+    </row>
+    <row r="23" spans="2:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="146" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="147"/>
+      <c r="E23" s="138" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="145"/>
+      <c r="G23" s="142" t="s">
+        <v>202</v>
+      </c>
+      <c r="H23" s="137"/>
+    </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="125"/>
+      <c r="C24" s="129" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="120" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="129" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="139" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="143" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="135"/>
       <c r="O24" s="55"/>
       <c r="P24" s="55"/>
     </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="126" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="130">
+        <v>156</v>
+      </c>
+      <c r="D25" s="123">
+        <f>C25/C29</f>
+        <v>0.1900121802679659</v>
+      </c>
+      <c r="E25" s="123">
+        <v>35</v>
+      </c>
+      <c r="F25" s="140">
+        <f>E25/E29</f>
+        <v>0.18041237113402062</v>
+      </c>
+      <c r="G25" s="143">
+        <v>1</v>
+      </c>
+      <c r="H25" s="135"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="126" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="131">
+        <v>139</v>
+      </c>
+      <c r="D26" s="123">
+        <f>C26/C29</f>
+        <v>0.16930572472594396</v>
+      </c>
+      <c r="E26" s="124">
+        <v>34</v>
+      </c>
+      <c r="F26" s="140">
+        <f>E26/E29</f>
+        <v>0.17525773195876287</v>
+      </c>
+      <c r="G26" s="143">
+        <v>1</v>
+      </c>
+      <c r="H26" s="135"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="126" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="130">
+        <v>172</v>
+      </c>
+      <c r="D27" s="123">
+        <f>C27/C29</f>
+        <v>0.20950060901339829</v>
+      </c>
+      <c r="E27" s="123">
+        <v>58</v>
+      </c>
+      <c r="F27" s="140">
+        <f>E27/E29</f>
+        <v>0.29896907216494845</v>
+      </c>
+      <c r="G27" s="143">
+        <v>4</v>
+      </c>
+      <c r="H27" s="135"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="127" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="132">
+        <v>354</v>
+      </c>
+      <c r="D28" s="118">
+        <f>C28/C29</f>
+        <v>0.43118148599269185</v>
+      </c>
+      <c r="E28" s="119">
+        <v>67</v>
+      </c>
+      <c r="F28" s="134">
+        <f>E28/E29</f>
+        <v>0.34536082474226804</v>
+      </c>
+      <c r="G28" s="143">
+        <v>4</v>
+      </c>
+      <c r="H28" s="135"/>
+    </row>
+    <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="128" t="s">
+        <v>200</v>
+      </c>
+      <c r="C29" s="133">
+        <f>SUM(C25:C28)</f>
+        <v>821</v>
+      </c>
+      <c r="D29" s="122" t="s">
+        <v>201</v>
+      </c>
+      <c r="E29" s="121">
+        <f>SUM(E25:E28)</f>
+        <v>194</v>
+      </c>
+      <c r="F29" s="141" t="s">
+        <v>201</v>
+      </c>
+      <c r="G29" s="144"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="D4:G4"/>
@@ -3076,7 +3428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:X62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
@@ -3100,79 +3452,79 @@
     </row>
     <row r="3" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="87"/>
-      <c r="C4" s="90" t="s">
+      <c r="B4" s="99"/>
+      <c r="C4" s="112" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="80"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="80"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="80"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="92"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="92"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="112"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="90"/>
+      <c r="X4" s="92"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="88"/>
-      <c r="C5" s="99" t="s">
+      <c r="B5" s="100"/>
+      <c r="C5" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101" t="s">
+      <c r="D5" s="117"/>
+      <c r="E5" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="102"/>
-      <c r="G5" s="95" t="s">
+      <c r="F5" s="109"/>
+      <c r="G5" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="J5" s="88"/>
-      <c r="K5" s="99" t="s">
+      <c r="J5" s="100"/>
+      <c r="K5" s="116" t="s">
         <v>182</v>
       </c>
-      <c r="L5" s="100"/>
-      <c r="M5" s="101" t="s">
+      <c r="L5" s="117"/>
+      <c r="M5" s="108" t="s">
         <v>184</v>
       </c>
-      <c r="N5" s="102"/>
-      <c r="O5" s="95" t="s">
+      <c r="N5" s="109"/>
+      <c r="O5" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="P5" s="97" t="s">
+      <c r="P5" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="R5" s="88"/>
-      <c r="S5" s="99" t="s">
+      <c r="R5" s="100"/>
+      <c r="S5" s="116" t="s">
         <v>183</v>
       </c>
-      <c r="T5" s="100"/>
-      <c r="U5" s="101" t="s">
+      <c r="T5" s="117"/>
+      <c r="U5" s="108" t="s">
         <v>185</v>
       </c>
-      <c r="V5" s="102"/>
-      <c r="W5" s="95" t="s">
+      <c r="V5" s="109"/>
+      <c r="W5" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="X5" s="97" t="s">
+      <c r="X5" s="110" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="89"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="42" t="s">
         <v>6</v>
       </c>
@@ -3185,9 +3537,9 @@
       <c r="F6" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="98"/>
-      <c r="J6" s="89"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="111"/>
+      <c r="J6" s="101"/>
       <c r="K6" s="65" t="s">
         <v>6</v>
       </c>
@@ -3200,9 +3552,9 @@
       <c r="N6" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="96"/>
-      <c r="P6" s="98"/>
-      <c r="R6" s="89"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="111"/>
+      <c r="R6" s="101"/>
       <c r="S6" s="42" t="s">
         <v>6</v>
       </c>
@@ -3215,8 +3567,8 @@
       <c r="V6" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="W6" s="96"/>
-      <c r="X6" s="98"/>
+      <c r="W6" s="103"/>
+      <c r="X6" s="111"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
@@ -3246,7 +3598,7 @@
       <c r="K7" s="37">
         <v>283</v>
       </c>
-      <c r="L7" s="107">
+      <c r="L7" s="73">
         <v>44.0809968847352</v>
       </c>
       <c r="M7" s="37">
@@ -3308,22 +3660,22 @@
       <c r="J8" s="62" t="s">
         <v>159</v>
       </c>
-      <c r="K8" s="115">
+      <c r="K8" s="81">
         <v>119</v>
       </c>
-      <c r="L8" s="116">
+      <c r="L8" s="82">
         <v>18.535825545171299</v>
       </c>
-      <c r="M8" s="115">
+      <c r="M8" s="81">
         <v>328</v>
       </c>
-      <c r="N8" s="117">
+      <c r="N8" s="83">
         <v>22.481151473612002</v>
       </c>
-      <c r="O8" s="111">
+      <c r="O8" s="77">
         <v>0.78457422002518296</v>
       </c>
-      <c r="P8" s="111">
+      <c r="P8" s="77">
         <v>4.2927158224870199E-2</v>
       </c>
       <c r="R8" s="30" t="s">
@@ -3394,22 +3746,22 @@
       <c r="R9" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="S9" s="108">
+      <c r="S9" s="74">
         <v>157</v>
       </c>
-      <c r="T9" s="109">
+      <c r="T9" s="75">
         <v>9.0699017908723292</v>
       </c>
-      <c r="U9" s="110">
+      <c r="U9" s="76">
         <v>744</v>
       </c>
-      <c r="V9" s="110">
+      <c r="V9" s="76">
         <v>11.5869802211493</v>
       </c>
-      <c r="W9" s="111">
+      <c r="W9" s="77">
         <v>0.76109852987389104</v>
       </c>
-      <c r="X9" s="111">
+      <c r="X9" s="77">
         <v>2.85987048958064E-3</v>
       </c>
     </row>
@@ -3589,51 +3941,51 @@
       <c r="R12" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="S12" s="112">
+      <c r="S12" s="78">
         <v>49</v>
       </c>
-      <c r="T12" s="113">
+      <c r="T12" s="79">
         <v>2.8307336799537799</v>
       </c>
-      <c r="U12" s="114">
+      <c r="U12" s="80">
         <v>121</v>
       </c>
-      <c r="V12" s="114">
+      <c r="V12" s="80">
         <v>1.8844416757514399</v>
       </c>
-      <c r="W12" s="111">
+      <c r="W12" s="77">
         <v>1.5167893397273999</v>
       </c>
-      <c r="X12" s="111">
+      <c r="X12" s="77">
         <v>1.7608763137178698E-2</v>
       </c>
     </row>
     <row r="13" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="87"/>
-      <c r="C14" s="90" t="s">
+      <c r="B14" s="99"/>
+      <c r="C14" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="80"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="92"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="88"/>
-      <c r="C15" s="99" t="s">
+      <c r="B15" s="100"/>
+      <c r="C15" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="102"/>
-      <c r="E15" s="101" t="s">
+      <c r="D15" s="109"/>
+      <c r="E15" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="102"/>
-      <c r="G15" s="103" t="s">
+      <c r="F15" s="109"/>
+      <c r="G15" s="113" t="s">
         <v>157</v>
       </c>
-      <c r="H15" s="105" t="s">
+      <c r="H15" s="115" t="s">
         <v>156</v>
       </c>
       <c r="O15" t="s">
@@ -3644,7 +3996,7 @@
       </c>
     </row>
     <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="89"/>
+      <c r="B16" s="101"/>
       <c r="C16" s="42" t="s">
         <v>6</v>
       </c>
@@ -3657,8 +4009,8 @@
       <c r="F16" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="104"/>
-      <c r="H16" s="98"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="111"/>
       <c r="N16" t="s">
         <v>186</v>
       </c>
@@ -3839,50 +4191,50 @@
     </row>
     <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="87"/>
-      <c r="C24" s="90" t="s">
+      <c r="B24" s="99"/>
+      <c r="C24" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="80"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="90"/>
+      <c r="L24" s="92"/>
       <c r="N24" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="88"/>
-      <c r="C25" s="91" t="s">
+      <c r="B25" s="100"/>
+      <c r="C25" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="92"/>
-      <c r="E25" s="93" t="s">
+      <c r="D25" s="105"/>
+      <c r="E25" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="F25" s="94"/>
-      <c r="G25" s="91" t="s">
+      <c r="F25" s="107"/>
+      <c r="G25" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="H25" s="92"/>
-      <c r="I25" s="93" t="s">
+      <c r="H25" s="105"/>
+      <c r="I25" s="106" t="s">
         <v>168</v>
       </c>
-      <c r="J25" s="94"/>
-      <c r="K25" s="95" t="s">
+      <c r="J25" s="107"/>
+      <c r="K25" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="L25" s="97" t="s">
+      <c r="L25" s="110" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="89"/>
+      <c r="B26" s="101"/>
       <c r="C26" s="44" t="s">
         <v>6</v>
       </c>
@@ -3907,8 +4259,8 @@
       <c r="J26" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="K26" s="96"/>
-      <c r="L26" s="98"/>
+      <c r="K26" s="103"/>
+      <c r="L26" s="111"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="32" t="s">
@@ -4097,83 +4449,83 @@
     </row>
     <row r="33" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B34" s="87"/>
-      <c r="C34" s="90" t="s">
+      <c r="B34" s="99"/>
+      <c r="C34" s="112" t="s">
         <v>177</v>
       </c>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="80"/>
-      <c r="N34" s="87"/>
-      <c r="O34" s="90" t="s">
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="H34" s="90"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="92"/>
+      <c r="N34" s="99"/>
+      <c r="O34" s="112" t="s">
         <v>178</v>
       </c>
-      <c r="P34" s="78"/>
-      <c r="Q34" s="78"/>
-      <c r="R34" s="78"/>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="78"/>
-      <c r="V34" s="78"/>
-      <c r="W34" s="78"/>
-      <c r="X34" s="80"/>
+      <c r="P34" s="90"/>
+      <c r="Q34" s="90"/>
+      <c r="R34" s="90"/>
+      <c r="S34" s="90"/>
+      <c r="T34" s="90"/>
+      <c r="U34" s="90"/>
+      <c r="V34" s="90"/>
+      <c r="W34" s="90"/>
+      <c r="X34" s="92"/>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B35" s="88"/>
-      <c r="C35" s="91" t="s">
+      <c r="B35" s="100"/>
+      <c r="C35" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="92"/>
-      <c r="E35" s="93" t="s">
+      <c r="D35" s="105"/>
+      <c r="E35" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="F35" s="94"/>
-      <c r="G35" s="91" t="s">
+      <c r="F35" s="107"/>
+      <c r="G35" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="H35" s="92"/>
-      <c r="I35" s="93" t="s">
+      <c r="H35" s="105"/>
+      <c r="I35" s="106" t="s">
         <v>168</v>
       </c>
-      <c r="J35" s="94"/>
-      <c r="K35" s="95" t="s">
+      <c r="J35" s="107"/>
+      <c r="K35" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="L35" s="97" t="s">
+      <c r="L35" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="N35" s="88"/>
-      <c r="O35" s="91" t="s">
+      <c r="N35" s="100"/>
+      <c r="O35" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="P35" s="92"/>
-      <c r="Q35" s="93" t="s">
+      <c r="P35" s="105"/>
+      <c r="Q35" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="R35" s="94"/>
-      <c r="S35" s="91" t="s">
+      <c r="R35" s="107"/>
+      <c r="S35" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="T35" s="92"/>
-      <c r="U35" s="93" t="s">
+      <c r="T35" s="105"/>
+      <c r="U35" s="106" t="s">
         <v>168</v>
       </c>
-      <c r="V35" s="94"/>
-      <c r="W35" s="95" t="s">
+      <c r="V35" s="107"/>
+      <c r="W35" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="X35" s="97" t="s">
+      <c r="X35" s="110" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="36" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="89"/>
+      <c r="B36" s="101"/>
       <c r="C36" s="44" t="s">
         <v>6</v>
       </c>
@@ -4198,9 +4550,9 @@
       <c r="J36" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="K36" s="96"/>
-      <c r="L36" s="98"/>
-      <c r="N36" s="89"/>
+      <c r="K36" s="103"/>
+      <c r="L36" s="111"/>
+      <c r="N36" s="101"/>
       <c r="O36" s="44" t="s">
         <v>6</v>
       </c>
@@ -4225,8 +4577,8 @@
       <c r="V36" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="W36" s="96"/>
-      <c r="X36" s="98"/>
+      <c r="W36" s="103"/>
+      <c r="X36" s="111"/>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" s="32" t="s">
@@ -4530,10 +4882,10 @@
       <c r="B42" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="C42" s="106">
+      <c r="C42" s="72">
         <v>13</v>
       </c>
-      <c r="D42" s="106">
+      <c r="D42" s="72">
         <v>3.25</v>
       </c>
       <c r="E42">
@@ -4559,10 +4911,10 @@
       <c r="N42" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="O42" s="106">
+      <c r="O42" s="72">
         <v>27</v>
       </c>
-      <c r="P42" s="106">
+      <c r="P42" s="72">
         <v>1.70562223626026</v>
       </c>
       <c r="Q42">
@@ -4588,83 +4940,83 @@
     </row>
     <row r="43" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B44" s="87"/>
-      <c r="C44" s="90" t="s">
+      <c r="B44" s="99"/>
+      <c r="C44" s="112" t="s">
         <v>199</v>
       </c>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="78"/>
-      <c r="L44" s="80"/>
-      <c r="N44" s="87"/>
-      <c r="O44" s="90" t="s">
+      <c r="D44" s="90"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="90"/>
+      <c r="G44" s="90"/>
+      <c r="H44" s="90"/>
+      <c r="I44" s="90"/>
+      <c r="J44" s="90"/>
+      <c r="K44" s="90"/>
+      <c r="L44" s="92"/>
+      <c r="N44" s="99"/>
+      <c r="O44" s="112" t="s">
         <v>179</v>
       </c>
-      <c r="P44" s="78"/>
-      <c r="Q44" s="78"/>
-      <c r="R44" s="78"/>
-      <c r="S44" s="78"/>
-      <c r="T44" s="78"/>
-      <c r="U44" s="78"/>
-      <c r="V44" s="78"/>
-      <c r="W44" s="78"/>
-      <c r="X44" s="80"/>
+      <c r="P44" s="90"/>
+      <c r="Q44" s="90"/>
+      <c r="R44" s="90"/>
+      <c r="S44" s="90"/>
+      <c r="T44" s="90"/>
+      <c r="U44" s="90"/>
+      <c r="V44" s="90"/>
+      <c r="W44" s="90"/>
+      <c r="X44" s="92"/>
     </row>
     <row r="45" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B45" s="88"/>
-      <c r="C45" s="91" t="s">
+      <c r="B45" s="100"/>
+      <c r="C45" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="D45" s="92"/>
-      <c r="E45" s="93" t="s">
+      <c r="D45" s="105"/>
+      <c r="E45" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="F45" s="94"/>
-      <c r="G45" s="91" t="s">
+      <c r="F45" s="107"/>
+      <c r="G45" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="H45" s="92"/>
-      <c r="I45" s="93" t="s">
+      <c r="H45" s="105"/>
+      <c r="I45" s="106" t="s">
         <v>168</v>
       </c>
-      <c r="J45" s="94"/>
-      <c r="K45" s="95" t="s">
+      <c r="J45" s="107"/>
+      <c r="K45" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="L45" s="97" t="s">
+      <c r="L45" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="N45" s="88"/>
-      <c r="O45" s="91" t="s">
+      <c r="N45" s="100"/>
+      <c r="O45" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="P45" s="92"/>
-      <c r="Q45" s="93" t="s">
+      <c r="P45" s="105"/>
+      <c r="Q45" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="R45" s="94"/>
-      <c r="S45" s="91" t="s">
+      <c r="R45" s="107"/>
+      <c r="S45" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="T45" s="92"/>
-      <c r="U45" s="93" t="s">
+      <c r="T45" s="105"/>
+      <c r="U45" s="106" t="s">
         <v>168</v>
       </c>
-      <c r="V45" s="94"/>
-      <c r="W45" s="95" t="s">
+      <c r="V45" s="107"/>
+      <c r="W45" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="X45" s="97" t="s">
+      <c r="X45" s="110" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="46" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="89"/>
+      <c r="B46" s="101"/>
       <c r="C46" s="44" t="s">
         <v>6</v>
       </c>
@@ -4689,9 +5041,9 @@
       <c r="J46" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="K46" s="96"/>
-      <c r="L46" s="98"/>
-      <c r="N46" s="89"/>
+      <c r="K46" s="103"/>
+      <c r="L46" s="111"/>
+      <c r="N46" s="101"/>
       <c r="O46" s="44" t="s">
         <v>6</v>
       </c>
@@ -4716,8 +5068,8 @@
       <c r="V46" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="W46" s="96"/>
-      <c r="X46" s="98"/>
+      <c r="W46" s="103"/>
+      <c r="X46" s="111"/>
     </row>
     <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B47" s="32" t="s">
@@ -5081,83 +5433,83 @@
       <c r="F53" s="29"/>
     </row>
     <row r="54" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B54" s="87"/>
-      <c r="C54" s="90" t="s">
+      <c r="B54" s="99"/>
+      <c r="C54" s="112" t="s">
         <v>180</v>
       </c>
-      <c r="D54" s="78"/>
-      <c r="E54" s="78"/>
-      <c r="F54" s="78"/>
-      <c r="G54" s="78"/>
-      <c r="H54" s="78"/>
-      <c r="I54" s="78"/>
-      <c r="J54" s="78"/>
-      <c r="K54" s="78"/>
-      <c r="L54" s="80"/>
-      <c r="N54" s="87"/>
-      <c r="O54" s="90" t="s">
+      <c r="D54" s="90"/>
+      <c r="E54" s="90"/>
+      <c r="F54" s="90"/>
+      <c r="G54" s="90"/>
+      <c r="H54" s="90"/>
+      <c r="I54" s="90"/>
+      <c r="J54" s="90"/>
+      <c r="K54" s="90"/>
+      <c r="L54" s="92"/>
+      <c r="N54" s="99"/>
+      <c r="O54" s="112" t="s">
         <v>181</v>
       </c>
-      <c r="P54" s="78"/>
-      <c r="Q54" s="78"/>
-      <c r="R54" s="78"/>
-      <c r="S54" s="78"/>
-      <c r="T54" s="78"/>
-      <c r="U54" s="78"/>
-      <c r="V54" s="78"/>
-      <c r="W54" s="78"/>
-      <c r="X54" s="80"/>
+      <c r="P54" s="90"/>
+      <c r="Q54" s="90"/>
+      <c r="R54" s="90"/>
+      <c r="S54" s="90"/>
+      <c r="T54" s="90"/>
+      <c r="U54" s="90"/>
+      <c r="V54" s="90"/>
+      <c r="W54" s="90"/>
+      <c r="X54" s="92"/>
     </row>
     <row r="55" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B55" s="88"/>
-      <c r="C55" s="91" t="s">
+      <c r="B55" s="100"/>
+      <c r="C55" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="92"/>
-      <c r="E55" s="93" t="s">
+      <c r="D55" s="105"/>
+      <c r="E55" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="F55" s="94"/>
-      <c r="G55" s="91" t="s">
+      <c r="F55" s="107"/>
+      <c r="G55" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="H55" s="92"/>
-      <c r="I55" s="93" t="s">
+      <c r="H55" s="105"/>
+      <c r="I55" s="106" t="s">
         <v>168</v>
       </c>
-      <c r="J55" s="94"/>
-      <c r="K55" s="95" t="s">
+      <c r="J55" s="107"/>
+      <c r="K55" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="L55" s="97" t="s">
+      <c r="L55" s="110" t="s">
         <v>156</v>
       </c>
-      <c r="N55" s="88"/>
-      <c r="O55" s="91" t="s">
+      <c r="N55" s="100"/>
+      <c r="O55" s="104" t="s">
         <v>106</v>
       </c>
-      <c r="P55" s="92"/>
-      <c r="Q55" s="93" t="s">
+      <c r="P55" s="105"/>
+      <c r="Q55" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="R55" s="94"/>
-      <c r="S55" s="91" t="s">
+      <c r="R55" s="107"/>
+      <c r="S55" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="T55" s="92"/>
-      <c r="U55" s="93" t="s">
+      <c r="T55" s="105"/>
+      <c r="U55" s="106" t="s">
         <v>168</v>
       </c>
-      <c r="V55" s="94"/>
-      <c r="W55" s="95" t="s">
+      <c r="V55" s="107"/>
+      <c r="W55" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="X55" s="97" t="s">
+      <c r="X55" s="110" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="56" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="89"/>
+      <c r="B56" s="101"/>
       <c r="C56" s="44" t="s">
         <v>6</v>
       </c>
@@ -5182,9 +5534,9 @@
       <c r="J56" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="K56" s="96"/>
-      <c r="L56" s="98"/>
-      <c r="N56" s="89"/>
+      <c r="K56" s="103"/>
+      <c r="L56" s="111"/>
+      <c r="N56" s="101"/>
       <c r="O56" s="44" t="s">
         <v>6</v>
       </c>
@@ -5209,8 +5561,8 @@
       <c r="V56" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="W56" s="96"/>
-      <c r="X56" s="98"/>
+      <c r="W56" s="103"/>
+      <c r="X56" s="111"/>
     </row>
     <row r="57" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B57" s="32" t="s">
@@ -5572,11 +5924,65 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="N54:N56"/>
+    <mergeCell ref="O54:X54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:K56"/>
+    <mergeCell ref="L55:L56"/>
+    <mergeCell ref="O55:P55"/>
+    <mergeCell ref="Q55:R55"/>
+    <mergeCell ref="S55:T55"/>
+    <mergeCell ref="U55:V55"/>
+    <mergeCell ref="W55:W56"/>
+    <mergeCell ref="X55:X56"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:L44"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="O44:X44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="S45:T45"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="W45:W46"/>
+    <mergeCell ref="X45:X46"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="O34:X34"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="W35:W36"/>
+    <mergeCell ref="X35:X36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:L34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:X4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="L25:L26"/>
     <mergeCell ref="I25:J25"/>
@@ -5593,65 +5999,11 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="S4:X4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:L34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="O34:X34"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="U35:V35"/>
-    <mergeCell ref="W35:W36"/>
-    <mergeCell ref="X35:X36"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:L44"/>
-    <mergeCell ref="N44:N46"/>
-    <mergeCell ref="O44:X44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="S45:T45"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="W45:W46"/>
-    <mergeCell ref="X45:X46"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="N54:N56"/>
-    <mergeCell ref="O54:X54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:K56"/>
-    <mergeCell ref="L55:L56"/>
-    <mergeCell ref="O55:P55"/>
-    <mergeCell ref="Q55:R55"/>
-    <mergeCell ref="S55:T55"/>
-    <mergeCell ref="U55:V55"/>
-    <mergeCell ref="W55:W56"/>
-    <mergeCell ref="X55:X56"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" copies="2" r:id="rId1"/>

</xml_diff>